<commit_message>
actualizacion de table y word de metrica de no conformidades
</commit_message>
<xml_diff>
--- a/Area de proceso MA/TABME_V1.0_2017.xlsx
+++ b/Area de proceso MA/TABME_V1.0_2017.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jared/Desktop/documentationStaradmin/Area de proceso MA/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10180" yWindow="2520" windowWidth="20500" windowHeight="7660" activeTab="3"/>
+    <workbookView xWindow="10185" yWindow="2520" windowWidth="20505" windowHeight="7665" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tableros" sheetId="1" r:id="rId1"/>
@@ -19,15 +14,12 @@
     <sheet name="FMICIC" sheetId="10" state="hidden" r:id="rId5"/>
     <sheet name="Hoja1" sheetId="11" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -35,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="76">
   <si>
     <t xml:space="preserve">    EJR-SOFT</t>
   </si>
@@ -131,9 +123,6 @@
   </si>
   <si>
     <t>TABLERO DE METRICAS DE NUMERO DE N CONFORMIDADES QA DE PRODUCTO</t>
-  </si>
-  <si>
-    <t>TABLA DE INDICADORES PPQA</t>
   </si>
   <si>
     <t>POR REVISAR</t>
@@ -261,6 +250,12 @@
   <si>
     <t>TABLA DE INDICADORES FMEXRI</t>
   </si>
+  <si>
+    <t>TABLA DE INDICADORES FMNCONPRO</t>
+  </si>
+  <si>
+    <t>FMNCONPRO</t>
+  </si>
 </sst>
 </file>
 
@@ -269,7 +264,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1475,7 +1470,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.145282137746027"/>
-          <c:y val="0.0231481801368554"/>
+          <c:y val="2.3148180136855399E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1503,7 +1498,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES_tradnl"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1520,12 +1515,9 @@
             <c:strRef>
               <c:f>FMNCONPRO!$B$31:$C$31</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PPQA</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Numero de N conformidades QA del Producto</c:v>
+                  <c:v>FMNCONPRO Numero de N conformidades QA del Producto</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1576,7 +1568,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-ES_tradnl"/>
+                <a:endParaRPr lang="es-ES"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -1630,13 +1622,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>7.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1659,11 +1651,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2001434320"/>
-        <c:axId val="-2001583408"/>
+        <c:axId val="58148352"/>
+        <c:axId val="58479744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2001434320"/>
+        <c:axId val="58148352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1695,6 +1687,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1703,26 +1696,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-ES_tradnl"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1758,10 +1731,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2001583408"/>
+        <c:crossAx val="58479744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1769,7 +1742,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2001583408"/>
+        <c:axId val="58479744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1827,6 +1800,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1835,32 +1809,12 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-ES_tradnl"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2001434320"/>
+        <c:crossAx val="58148352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1914,7 +1868,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES_tradnl"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1969,8 +1923,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.105916666666667"/>
-          <c:y val="0.0416666666666667"/>
+          <c:x val="0.10591666666666701"/>
+          <c:y val="4.1666666666666699E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1981,26 +1935,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-ES_tradnl"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -2016,12 +1950,9 @@
             <c:strRef>
               <c:f>FMNCONPRO!$C$39:$C$40</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TABLERO DE METRICAS DE N CONFORMIDADES QA DE PRODUCTO</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>VALORES</c:v>
+                  <c:v>TABLERO DE METRICAS DE N CONFORMIDADES QA DE PRODUCTO VALORES</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2067,7 +1998,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-ES_tradnl"/>
+                <a:endParaRPr lang="es-ES"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="inEnd"/>
@@ -2121,13 +2052,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.636363636363636</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.459459459459459</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.157894736842105</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2148,11 +2079,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="-1962773856"/>
-        <c:axId val="-1962764720"/>
+        <c:axId val="61113856"/>
+        <c:axId val="61135104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1962773856"/>
+        <c:axId val="61113856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2192,10 +2123,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1962764720"/>
+        <c:crossAx val="61135104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2203,7 +2134,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1962764720"/>
+        <c:axId val="61135104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2224,7 +2155,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1962773856"/>
+        <c:crossAx val="61113856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2275,7 +2206,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES_tradnl"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2339,26 +2270,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-ES_tradnl"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -2367,10 +2278,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0595671478565179"/>
-          <c:y val="0.01497619546023"/>
-          <c:w val="0.837655074365704"/>
-          <c:h val="0.777796027030363"/>
+          <c:x val="5.9567147856517899E-2"/>
+          <c:y val="1.4976195460229999E-2"/>
+          <c:w val="0.83765507436570397"/>
+          <c:h val="0.77779602703036299"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2430,13 +2341,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2458,11 +2369,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1999700448"/>
-        <c:axId val="-1999865152"/>
+        <c:axId val="77250944"/>
+        <c:axId val="83642624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1999700448"/>
+        <c:axId val="77250944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2502,26 +2413,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-ES_tradnl"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2557,10 +2448,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1999865152"/>
+        <c:crossAx val="83642624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2568,7 +2459,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1999865152"/>
+        <c:axId val="83642624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2622,26 +2513,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-ES_tradnl"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2671,10 +2542,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1999700448"/>
+        <c:crossAx val="77250944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2716,7 +2587,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES_tradnl"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2743,7 +2614,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES_tradnl"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2773,8 +2644,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.119465223097113"/>
-          <c:y val="0.0231481481481481"/>
+          <c:x val="0.11946522309711299"/>
+          <c:y val="2.3148148148148098E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2802,7 +2673,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES_tradnl"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2859,12 +2730,9 @@
             <c:strRef>
               <c:f>FMVREQM!$B$46:$B$47</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TABLERO DE METRICAS DE N CONFORMIDADES QA DE PRODUCTO</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>VALORES</c:v>
+                  <c:v>TABLERO DE METRICAS DE N CONFORMIDADES QA DE PRODUCTO VALORES</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2904,13 +2772,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.66666666666666</c:v>
+                  <c:v>16.666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2931,12 +2799,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="-1962573040"/>
-        <c:axId val="-1962570720"/>
+        <c:axId val="139487104"/>
+        <c:axId val="139488640"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-1962573040"/>
+        <c:axId val="139487104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2970,10 +2838,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1962570720"/>
+        <c:crossAx val="139488640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2981,7 +2849,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1962570720"/>
+        <c:axId val="139488640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3026,10 +2894,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1962573040"/>
+        <c:crossAx val="139487104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3064,7 +2932,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES_tradnl"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3124,26 +2992,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-ES_tradnl"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -3200,7 +3048,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-ES_tradnl"/>
+                <a:endParaRPr lang="es-ES"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -3255,13 +3103,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3284,11 +3132,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1962501280"/>
-        <c:axId val="-1962497888"/>
+        <c:axId val="175112576"/>
+        <c:axId val="175134208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1962501280"/>
+        <c:axId val="175112576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3334,26 +3182,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-ES_tradnl"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -3389,10 +3217,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1962497888"/>
+        <c:crossAx val="175134208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3400,7 +3228,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1962497888"/>
+        <c:axId val="175134208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3457,32 +3285,12 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-ES_tradnl"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1962501280"/>
+        <c:crossAx val="175112576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3533,7 +3341,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES_tradnl"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3590,7 +3398,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3599,32 +3406,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-ES_tradnl"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -3710,13 +3491,13 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3737,11 +3518,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="-1999687904"/>
-        <c:axId val="-1999685360"/>
+        <c:axId val="189869056"/>
+        <c:axId val="189899136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1999687904"/>
+        <c:axId val="189869056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3772,7 +3553,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3781,25 +3561,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="85000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-ES_tradnl"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -3834,10 +3595,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1999685360"/>
+        <c:crossAx val="189899136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3845,7 +3606,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1999685360"/>
+        <c:axId val="189899136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3890,7 +3651,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3899,25 +3659,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="85000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-ES_tradnl"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -3946,10 +3687,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1999687904"/>
+        <c:crossAx val="189869056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4000,7 +3741,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES_tradnl"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4031,7 +3772,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.145282137746027"/>
-          <c:y val="0.0231481801368554"/>
+          <c:y val="2.3148180136855399E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -4059,7 +3800,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES_tradnl"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4076,12 +3817,9 @@
             <c:strRef>
               <c:f>FMICIC!$B$31:$C$31</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CM</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Numero de Items Modificados</c:v>
+                  <c:v>CM Numero de Items Modificados</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4132,7 +3870,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-ES_tradnl"/>
+                <a:endParaRPr lang="es-ES"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -4186,13 +3924,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4215,11 +3953,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1962388704"/>
-        <c:axId val="-1962384672"/>
+        <c:axId val="191199488"/>
+        <c:axId val="191686144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1962388704"/>
+        <c:axId val="191199488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4259,26 +3997,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-ES_tradnl"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -4314,10 +4032,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1962384672"/>
+        <c:crossAx val="191686144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4325,7 +4043,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1962384672"/>
+        <c:axId val="191686144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4391,32 +4109,12 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-ES_tradnl"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1962388704"/>
+        <c:crossAx val="191199488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4470,7 +4168,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES_tradnl"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4525,8 +4223,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.105916666666667"/>
-          <c:y val="0.0416666666666667"/>
+          <c:x val="0.10591666666666701"/>
+          <c:y val="4.1666666666666699E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -4537,26 +4235,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-ES_tradnl"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -4572,12 +4250,9 @@
             <c:strRef>
               <c:f>FMICIC!$C$39:$C$40</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TABLERO DE METRICAS DE N CONFORMIDADES QA DE PRODUCTO</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>VALORES</c:v>
+                  <c:v>TABLERO DE METRICAS DE N CONFORMIDADES QA DE PRODUCTO VALORES</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4623,7 +4298,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-ES_tradnl"/>
+                <a:endParaRPr lang="es-ES"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="inEnd"/>
@@ -4677,13 +4352,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.216216216216216</c:v>
+                  <c:v>0.21621621621621623</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4704,11 +4379,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="-1962358400"/>
-        <c:axId val="-1962355648"/>
+        <c:axId val="201783552"/>
+        <c:axId val="77283328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1962358400"/>
+        <c:axId val="201783552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4748,10 +4423,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1962355648"/>
+        <c:crossAx val="77283328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4759,7 +4434,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1962355648"/>
+        <c:axId val="77283328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4780,7 +4455,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1962358400"/>
+        <c:crossAx val="201783552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4831,7 +4506,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES_tradnl"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -10488,7 +10163,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -10500,22 +10175,22 @@
   <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="9" max="9" width="7.6640625" customWidth="1"/>
-    <col min="10" max="10" width="17.33203125" customWidth="1"/>
-    <col min="11" max="11" width="24.83203125" customWidth="1"/>
-    <col min="15" max="16" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" customWidth="1"/>
+    <col min="15" max="16" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="15" customHeight="1">
       <c r="A1" s="100" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B1" s="101"/>
       <c r="C1" s="101"/>
@@ -10533,7 +10208,7 @@
       <c r="O1" s="101"/>
       <c r="P1" s="102"/>
     </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="15" customHeight="1">
       <c r="A2" s="103"/>
       <c r="B2" s="104"/>
       <c r="C2" s="104"/>
@@ -10551,7 +10226,7 @@
       <c r="O2" s="104"/>
       <c r="P2" s="105"/>
     </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="15" customHeight="1">
       <c r="A3" s="103"/>
       <c r="B3" s="104"/>
       <c r="C3" s="104"/>
@@ -10569,7 +10244,7 @@
       <c r="O3" s="104"/>
       <c r="P3" s="105"/>
     </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="15" customHeight="1">
       <c r="A4" s="103"/>
       <c r="B4" s="104"/>
       <c r="C4" s="104"/>
@@ -10587,7 +10262,7 @@
       <c r="O4" s="104"/>
       <c r="P4" s="105"/>
     </row>
-    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="15.75" customHeight="1">
       <c r="A5" s="103"/>
       <c r="B5" s="104"/>
       <c r="C5" s="104"/>
@@ -10605,7 +10280,7 @@
       <c r="O5" s="104"/>
       <c r="P5" s="105"/>
     </row>
-    <row r="6" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="15.75" customHeight="1" thickBot="1">
       <c r="A6" s="106"/>
       <c r="B6" s="107"/>
       <c r="C6" s="107"/>
@@ -10623,9 +10298,9 @@
       <c r="O6" s="107"/>
       <c r="P6" s="108"/>
     </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="15" customHeight="1">
       <c r="A7" s="109" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" s="110"/>
       <c r="C7" s="110"/>
@@ -10643,7 +10318,7 @@
       <c r="O7" s="110"/>
       <c r="P7" s="111"/>
     </row>
-    <row r="8" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="15.75" customHeight="1" thickBot="1">
       <c r="A8" s="112"/>
       <c r="B8" s="113"/>
       <c r="C8" s="113"/>
@@ -10661,7 +10336,7 @@
       <c r="O8" s="113"/>
       <c r="P8" s="114"/>
     </row>
-    <row r="9" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="15.95" thickBot="1">
       <c r="A9" s="19"/>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
@@ -10672,12 +10347,12 @@
       <c r="H9" s="16"/>
       <c r="I9" s="16"/>
     </row>
-    <row r="10" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="15.95" thickBot="1">
       <c r="A10" s="79" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="119" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" s="120"/>
       <c r="D10" s="120"/>
@@ -10687,7 +10362,7 @@
       <c r="H10" s="120"/>
       <c r="I10" s="121"/>
     </row>
-    <row r="11" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="17.100000000000001" thickBot="1">
       <c r="A11" s="122" t="s">
         <v>27</v>
       </c>
@@ -10700,7 +10375,7 @@
       <c r="H11" s="123"/>
       <c r="I11" s="124"/>
     </row>
-    <row r="12" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="15.95" thickBot="1">
       <c r="A12" s="80"/>
       <c r="B12" s="115" t="s">
         <v>5</v>
@@ -10719,7 +10394,7 @@
       </c>
       <c r="I12" s="117"/>
     </row>
-    <row r="13" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="26.25" thickBot="1">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -10748,7 +10423,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="15.95" thickBot="1">
       <c r="A14" s="3" t="s">
         <v>22</v>
       </c>
@@ -10762,7 +10437,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F14" s="4">
         <v>0</v>
@@ -10777,7 +10452,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="15.95" thickBot="1">
       <c r="A15" s="7" t="s">
         <v>23</v>
       </c>
@@ -10788,7 +10463,7 @@
         <v>5</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E15" s="4">
         <v>1</v>
@@ -10806,7 +10481,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="15.95" thickBot="1">
       <c r="A16" s="10" t="s">
         <v>24</v>
       </c>
@@ -10817,10 +10492,10 @@
         <v>25</v>
       </c>
       <c r="D16" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="F16" s="4">
         <v>36</v>
@@ -10835,7 +10510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="15.95" thickBot="1">
       <c r="A17" s="19"/>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
@@ -10846,7 +10521,7 @@
       <c r="H17" s="16"/>
       <c r="I17" s="16"/>
     </row>
-    <row r="18" spans="1:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" ht="20.100000000000001" thickBot="1">
       <c r="J18" s="97" t="s">
         <v>26</v>
       </c>
@@ -10857,7 +10532,7 @@
       <c r="O18" s="98"/>
       <c r="P18" s="99"/>
     </row>
-    <row r="19" spans="1:16" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" ht="32.25" customHeight="1">
       <c r="J19" s="17" t="s">
         <v>3</v>
       </c>
@@ -10880,7 +10555,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" ht="29.25" customHeight="1">
       <c r="J20" s="14" t="s">
         <v>5</v>
       </c>
@@ -10889,15 +10564,15 @@
       </c>
       <c r="L20" s="88">
         <f>FMNCONPRO!D33</f>
-        <v>0.63636363636363635</v>
+        <v>0</v>
       </c>
       <c r="M20" s="88">
         <f>FMNCONPRO!E33</f>
-        <v>0.45945945945945948</v>
+        <v>0.2</v>
       </c>
       <c r="N20" s="88">
         <f>FMNCONPRO!F33</f>
-        <v>0.15789473684210525</v>
+        <v>0</v>
       </c>
       <c r="O20" s="13">
         <f>FMNCONPRO!G33</f>
@@ -10905,10 +10580,10 @@
       </c>
       <c r="P20" s="88">
         <f>FMNCONPRO!H33</f>
-        <v>0.41790594422173372</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="0.75" hidden="1" customHeight="1">
       <c r="J21" s="14" t="s">
         <v>6</v>
       </c>
@@ -10936,7 +10611,7 @@
         <v>7.2072072072072071E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" ht="30" customHeight="1">
       <c r="J22" s="14" t="s">
         <v>7</v>
       </c>
@@ -10964,7 +10639,7 @@
         <v>8.3333333333333321</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" ht="30" customHeight="1">
       <c r="J23" s="14" t="s">
         <v>8</v>
       </c>
@@ -10992,7 +10667,7 @@
         <v>14.333333333333334</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16">
       <c r="J24" s="11"/>
       <c r="K24" s="11"/>
       <c r="L24" s="11"/>
@@ -11105,27 +10780,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="11.5" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" customWidth="1"/>
-    <col min="6" max="6" width="8.1640625" customWidth="1"/>
-    <col min="7" max="7" width="11.1640625" customWidth="1"/>
-    <col min="8" max="8" width="9.5" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" customWidth="1"/>
-    <col min="10" max="10" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="15" customHeight="1">
       <c r="A1" s="100" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B1" s="101"/>
       <c r="C1" s="101"/>
@@ -11145,7 +10820,7 @@
       <c r="Q1" s="33"/>
       <c r="R1" s="33"/>
     </row>
-    <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="15" customHeight="1">
       <c r="A2" s="103"/>
       <c r="B2" s="104"/>
       <c r="C2" s="104"/>
@@ -11165,7 +10840,7 @@
       <c r="Q2" s="33"/>
       <c r="R2" s="33"/>
     </row>
-    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="15" customHeight="1">
       <c r="A3" s="103"/>
       <c r="B3" s="104"/>
       <c r="C3" s="104"/>
@@ -11185,7 +10860,7 @@
       <c r="Q3" s="33"/>
       <c r="R3" s="33"/>
     </row>
-    <row r="4" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="15" customHeight="1">
       <c r="A4" s="103"/>
       <c r="B4" s="104"/>
       <c r="C4" s="104"/>
@@ -11205,7 +10880,7 @@
       <c r="Q4" s="33"/>
       <c r="R4" s="33"/>
     </row>
-    <row r="5" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="15.75" customHeight="1">
       <c r="A5" s="103"/>
       <c r="B5" s="104"/>
       <c r="C5" s="104"/>
@@ -11225,7 +10900,7 @@
       <c r="Q5" s="33"/>
       <c r="R5" s="33"/>
     </row>
-    <row r="6" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
       <c r="A6" s="106"/>
       <c r="B6" s="107"/>
       <c r="C6" s="107"/>
@@ -11245,20 +10920,20 @@
       <c r="Q6" s="33"/>
       <c r="R6" s="33"/>
     </row>
-    <row r="7" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="15.95" thickBot="1"/>
+    <row r="8" spans="1:18">
       <c r="C8" s="125" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="D8" s="126"/>
       <c r="E8" s="127"/>
     </row>
-    <row r="9" spans="1:18" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="23.25" customHeight="1" thickBot="1">
       <c r="C9" s="128"/>
       <c r="D9" s="129"/>
       <c r="E9" s="130"/>
     </row>
-    <row r="10" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="26.25" thickBot="1">
       <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
@@ -11269,7 +10944,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="15.95" thickBot="1">
       <c r="C11" s="3" t="s">
         <v>22</v>
       </c>
@@ -11280,7 +10955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="15.95" thickBot="1">
       <c r="C12" s="7" t="s">
         <v>23</v>
       </c>
@@ -11291,7 +10966,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="15.95" thickBot="1">
       <c r="C13" s="10" t="s">
         <v>24</v>
       </c>
@@ -11302,8 +10977,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:18" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="15.95" thickBot="1"/>
+    <row r="15" spans="1:18" ht="32.25" customHeight="1" thickBot="1">
       <c r="A15" s="133" t="s">
         <v>31</v>
       </c>
@@ -11317,24 +10992,24 @@
       <c r="I15" s="48"/>
       <c r="J15" s="48"/>
     </row>
-    <row r="16" spans="1:18" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="60.75" thickBot="1">
       <c r="A16" s="37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="38" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="40" t="s">
+      <c r="F16" s="40" t="s">
         <v>43</v>
-      </c>
-      <c r="F16" s="40" t="s">
-        <v>44</v>
       </c>
       <c r="G16" s="40" t="s">
         <v>17</v>
@@ -11343,12 +11018,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="43" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="42.95" customHeight="1" thickBot="1">
       <c r="A17" s="42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B17" s="43" t="s">
-        <v>5</v>
+        <v>75</v>
       </c>
       <c r="C17" s="44" t="s">
         <v>9</v>
@@ -11357,22 +11032,22 @@
         <v>13</v>
       </c>
       <c r="E17" s="45">
+        <v>0</v>
+      </c>
+      <c r="F17" s="45">
         <v>7</v>
-      </c>
-      <c r="F17" s="45">
-        <v>11</v>
       </c>
       <c r="G17" s="46">
         <f>E17/F17</f>
-        <v>0.63636363636363635</v>
+        <v>0</v>
       </c>
       <c r="H17" s="47">
         <f>+G17</f>
-        <v>0.63636363636363635</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" thickBot="1"/>
+    <row r="20" spans="1:10" ht="30.75" customHeight="1" thickBot="1">
       <c r="A20" s="133" t="s">
         <v>31</v>
       </c>
@@ -11384,24 +11059,24 @@
       <c r="G20" s="134"/>
       <c r="H20" s="134"/>
     </row>
-    <row r="21" spans="1:10" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="60.75" thickBot="1">
       <c r="A21" s="37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" s="38" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D21" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="40" t="s">
+      <c r="F21" s="40" t="s">
         <v>43</v>
-      </c>
-      <c r="F21" s="40" t="s">
-        <v>44</v>
       </c>
       <c r="G21" s="40" t="s">
         <v>17</v>
@@ -11410,12 +11085,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="43" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="39" thickBot="1">
       <c r="A22" s="42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B22" s="43" t="s">
-        <v>5</v>
+        <v>75</v>
       </c>
       <c r="C22" s="44" t="s">
         <v>9</v>
@@ -11424,21 +11099,21 @@
         <v>14</v>
       </c>
       <c r="E22" s="45">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="F22" s="45">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="G22" s="46">
         <f>E22/F22</f>
-        <v>0.45945945945945948</v>
+        <v>0.2</v>
       </c>
       <c r="H22" s="47">
         <f>+G22</f>
-        <v>0.45945945945945948</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="33.75" customHeight="1" thickBot="1">
       <c r="A23" s="51"/>
       <c r="B23" s="84"/>
       <c r="C23" s="85"/>
@@ -11448,7 +11123,7 @@
       <c r="G23" s="87"/>
       <c r="H23" s="87"/>
     </row>
-    <row r="24" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="30.75" customHeight="1" thickBot="1">
       <c r="A24" s="133" t="s">
         <v>31</v>
       </c>
@@ -11460,24 +11135,24 @@
       <c r="G24" s="134"/>
       <c r="H24" s="134"/>
     </row>
-    <row r="25" spans="1:10" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="60.75" thickBot="1">
       <c r="A25" s="37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B25" s="77" t="s">
         <v>3</v>
       </c>
       <c r="C25" s="39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D25" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="40" t="s">
+      <c r="F25" s="40" t="s">
         <v>43</v>
-      </c>
-      <c r="F25" s="40" t="s">
-        <v>44</v>
       </c>
       <c r="G25" s="40" t="s">
         <v>17</v>
@@ -11486,12 +11161,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="43" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="39" thickBot="1">
       <c r="A26" s="42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B26" s="43" t="s">
-        <v>5</v>
+        <v>75</v>
       </c>
       <c r="C26" s="44" t="s">
         <v>9</v>
@@ -11500,21 +11175,21 @@
         <v>15</v>
       </c>
       <c r="E26" s="45">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F26" s="45">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G26" s="46">
         <f>E26/F26</f>
-        <v>0.15789473684210525</v>
+        <v>0</v>
       </c>
       <c r="H26" s="47">
         <f>+G26</f>
-        <v>0.15789473684210525</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="21" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="21">
       <c r="A27" s="51"/>
       <c r="B27" s="84"/>
       <c r="C27" s="85"/>
@@ -11524,8 +11199,8 @@
       <c r="G27" s="87"/>
       <c r="H27" s="87"/>
     </row>
-    <row r="28" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:10" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="15.75" thickBot="1"/>
+    <row r="29" spans="1:10" ht="42.75" customHeight="1" thickBot="1">
       <c r="A29" s="137" t="s">
         <v>31</v>
       </c>
@@ -11539,15 +11214,15 @@
       <c r="I29" s="48"/>
       <c r="J29" s="48"/>
     </row>
-    <row r="30" spans="1:10" s="31" customFormat="1" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" s="31" customFormat="1" ht="54.75" customHeight="1" thickBot="1">
       <c r="A30" s="53" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" s="54" t="s">
         <v>3</v>
       </c>
       <c r="C30" s="54" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D30" s="54" t="s">
         <v>13</v>
@@ -11563,33 +11238,33 @@
       <c r="I30" s="50"/>
       <c r="J30" s="50"/>
     </row>
-    <row r="31" spans="1:10" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="36" customHeight="1" thickBot="1">
       <c r="A31" s="42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>5</v>
+        <v>75</v>
       </c>
       <c r="C31" s="12" t="s">
         <v>9</v>
       </c>
       <c r="D31" s="13">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E31" s="13">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="F31" s="13">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G31" s="144"/>
       <c r="H31" s="145"/>
       <c r="I31" s="51"/>
       <c r="J31" s="52"/>
     </row>
-    <row r="32" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="24">
       <c r="A32" s="135" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B32" s="136"/>
       <c r="C32" s="136"/>
@@ -11597,35 +11272,35 @@
         <v>11</v>
       </c>
       <c r="E32" s="20">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="F32" s="13">
+        <v>29</v>
+      </c>
+      <c r="G32" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="G32" s="54" t="s">
-        <v>39</v>
-      </c>
       <c r="H32" s="56" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" ht="27" thickBot="1">
       <c r="A33" s="139" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B33" s="140"/>
       <c r="C33" s="141"/>
       <c r="D33" s="59">
         <f>D31/D32</f>
-        <v>0.63636363636363635</v>
+        <v>0</v>
       </c>
       <c r="E33" s="59">
         <f>E31/E32</f>
-        <v>0.45945945945945948</v>
+        <v>0.2</v>
       </c>
       <c r="F33" s="89">
         <f>F31/F32</f>
-        <v>0.15789473684210525</v>
+        <v>0</v>
       </c>
       <c r="G33" s="61">
         <f>+J33</f>
@@ -11633,14 +11308,14 @@
       </c>
       <c r="H33" s="62">
         <f>AVERAGE(D33:F33)</f>
-        <v>0.41790594422173372</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20">
       <c r="K34" s="58"/>
     </row>
-    <row r="38" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:20" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" ht="15.75" thickBot="1"/>
+    <row r="39" spans="1:20" ht="39.75" customHeight="1">
       <c r="B39" s="131" t="s">
         <v>28</v>
       </c>
@@ -11654,7 +11329,7 @@
       <c r="J39" s="21"/>
       <c r="T39" s="49"/>
     </row>
-    <row r="40" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:20" ht="15.75">
       <c r="B40" s="22" t="s">
         <v>30</v>
       </c>
@@ -11662,31 +11337,31 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20">
       <c r="B41" s="76" t="s">
         <v>13</v>
       </c>
       <c r="C41" s="36">
-        <f>D33</f>
-        <v>0.63636363636363635</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+        <f>D31/D32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20">
       <c r="B42" s="76" t="s">
         <v>14</v>
       </c>
       <c r="C42" s="36">
-        <f>E31/37</f>
-        <v>0.45945945945945948</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+        <f>E31/E32</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20">
       <c r="B43" s="76" t="s">
         <v>15</v>
       </c>
       <c r="C43" s="36">
         <f>F31/F32</f>
-        <v>0.15789473684210525</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -11826,17 +11501,17 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
-    <col min="6" max="6" width="10.5" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" s="100" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B1" s="101"/>
       <c r="C1" s="101"/>
@@ -11850,7 +11525,7 @@
       <c r="K1" s="101"/>
       <c r="L1" s="102"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" s="103"/>
       <c r="B2" s="104"/>
       <c r="C2" s="104"/>
@@ -11864,7 +11539,7 @@
       <c r="K2" s="104"/>
       <c r="L2" s="105"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" s="103"/>
       <c r="B3" s="104"/>
       <c r="C3" s="104"/>
@@ -11878,7 +11553,7 @@
       <c r="K3" s="104"/>
       <c r="L3" s="105"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4" s="103"/>
       <c r="B4" s="104"/>
       <c r="C4" s="104"/>
@@ -11892,7 +11567,7 @@
       <c r="K4" s="104"/>
       <c r="L4" s="105"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" s="103"/>
       <c r="B5" s="104"/>
       <c r="C5" s="104"/>
@@ -11906,7 +11581,7 @@
       <c r="K5" s="104"/>
       <c r="L5" s="105"/>
     </row>
-    <row r="6" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15.75" thickBot="1">
       <c r="A6" s="106"/>
       <c r="B6" s="107"/>
       <c r="C6" s="107"/>
@@ -11920,20 +11595,20 @@
       <c r="K6" s="107"/>
       <c r="L6" s="108"/>
     </row>
-    <row r="7" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="15.95" thickBot="1"/>
+    <row r="8" spans="1:12">
       <c r="A8" s="125" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8" s="126"/>
       <c r="C8" s="127"/>
     </row>
-    <row r="9" spans="1:12" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="33" customHeight="1" thickBot="1">
       <c r="A9" s="128"/>
       <c r="B9" s="129"/>
       <c r="C9" s="130"/>
     </row>
-    <row r="10" spans="1:12" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="26.25" thickBot="1">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -11944,7 +11619,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="15.95" thickBot="1">
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
@@ -11955,7 +11630,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="15.95" thickBot="1">
       <c r="A12" s="7" t="s">
         <v>23</v>
       </c>
@@ -11966,7 +11641,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="15.95" thickBot="1">
       <c r="A13" s="10" t="s">
         <v>24</v>
       </c>
@@ -11977,10 +11652,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:12" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="15.95" thickBot="1"/>
+    <row r="15" spans="1:12" ht="20.100000000000001" thickBot="1">
       <c r="A15" s="137" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" s="138"/>
       <c r="C15" s="138"/>
@@ -11992,18 +11667,18 @@
       <c r="I15" s="138"/>
       <c r="J15" s="146"/>
     </row>
-    <row r="16" spans="1:12" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="30.75" customHeight="1" thickBot="1">
       <c r="A16" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="29" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E16" s="29" t="s">
         <v>14</v>
@@ -12012,27 +11687,27 @@
         <v>15</v>
       </c>
       <c r="G16" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H16" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="I16" s="30" t="s">
+      <c r="J16" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="J16" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:10" ht="30.95" thickBot="1">
       <c r="A17" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B17" s="25" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" s="26">
         <v>0</v>
@@ -12041,7 +11716,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G17" s="26">
         <f>+H17</f>
@@ -12060,10 +11735,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:10" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="15.75" thickBot="1"/>
+    <row r="21" spans="1:10" ht="19.5" thickBot="1">
       <c r="A21" s="133" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21" s="134"/>
       <c r="C21" s="134"/>
@@ -12073,24 +11748,24 @@
       <c r="G21" s="134"/>
       <c r="H21" s="134"/>
     </row>
-    <row r="22" spans="1:10" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="48.75" thickBot="1">
       <c r="A22" s="37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="38" t="s">
         <v>3</v>
       </c>
       <c r="C22" s="63" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D22" s="40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E22" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" s="40" t="s">
         <v>47</v>
-      </c>
-      <c r="F22" s="40" t="s">
-        <v>48</v>
       </c>
       <c r="G22" s="40" t="s">
         <v>17</v>
@@ -12099,18 +11774,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="30.75" thickBot="1">
       <c r="A23" s="42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B23" s="43" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D23" s="45" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E23" s="45">
         <v>0</v>
@@ -12127,10 +11802,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:10" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="15.75" thickBot="1"/>
+    <row r="27" spans="1:10" ht="19.5" thickBot="1">
       <c r="A27" s="133" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B27" s="134"/>
       <c r="C27" s="134"/>
@@ -12140,24 +11815,24 @@
       <c r="G27" s="134"/>
       <c r="H27" s="134"/>
     </row>
-    <row r="28" spans="1:10" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="48.75" thickBot="1">
       <c r="A28" s="37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28" s="38" t="s">
         <v>3</v>
       </c>
       <c r="C28" s="63" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D28" s="40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E28" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" s="40" t="s">
         <v>47</v>
-      </c>
-      <c r="F28" s="40" t="s">
-        <v>48</v>
       </c>
       <c r="G28" s="40" t="s">
         <v>17</v>
@@ -12166,15 +11841,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="30.75" thickBot="1">
       <c r="A29" s="42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B29" s="43" t="s">
         <v>7</v>
       </c>
       <c r="C29" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D29" s="45" t="s">
         <v>14</v>
@@ -12194,7 +11869,7 @@
         <v>16.666666666666664</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="22" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="21.75" thickBot="1">
       <c r="A30" s="51"/>
       <c r="B30" s="84"/>
       <c r="C30" s="93"/>
@@ -12204,9 +11879,9 @@
       <c r="G30" s="94"/>
       <c r="H30" s="87"/>
     </row>
-    <row r="31" spans="1:10" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="19.5" thickBot="1">
       <c r="A31" s="133" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B31" s="134"/>
       <c r="C31" s="134"/>
@@ -12216,24 +11891,24 @@
       <c r="G31" s="134"/>
       <c r="H31" s="134"/>
     </row>
-    <row r="32" spans="1:10" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="48.75" thickBot="1">
       <c r="A32" s="37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32" s="90" t="s">
         <v>3</v>
       </c>
       <c r="C32" s="63" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D32" s="40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E32" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="F32" s="40" t="s">
         <v>47</v>
-      </c>
-      <c r="F32" s="40" t="s">
-        <v>48</v>
       </c>
       <c r="G32" s="40" t="s">
         <v>17</v>
@@ -12242,15 +11917,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="30.75" thickBot="1">
       <c r="A33" s="42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B33" s="43" t="s">
         <v>7</v>
       </c>
       <c r="C33" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D33" s="45" t="s">
         <v>15</v>
@@ -12270,14 +11945,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="15.75" thickBot="1">
       <c r="A38" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="19.5" thickBot="1">
       <c r="A39" s="137" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B39" s="138"/>
       <c r="C39" s="138"/>
@@ -12287,15 +11962,15 @@
       <c r="G39" s="138"/>
       <c r="H39" s="138"/>
     </row>
-    <row r="40" spans="1:8" ht="25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="24.75" thickBot="1">
       <c r="A40" s="53" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B40" s="54" t="s">
         <v>3</v>
       </c>
       <c r="C40" s="54" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D40" s="54" t="s">
         <v>13</v>
@@ -12309,15 +11984,15 @@
       <c r="G40" s="142"/>
       <c r="H40" s="143"/>
     </row>
-    <row r="41" spans="1:8" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="54" customHeight="1" thickBot="1">
       <c r="A41" s="95" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B41" s="43" t="s">
         <v>7</v>
       </c>
       <c r="C41" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D41" s="13">
         <v>0</v>
@@ -12331,9 +12006,9 @@
       <c r="G41" s="144"/>
       <c r="H41" s="145"/>
     </row>
-    <row r="42" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" ht="24">
       <c r="A42" s="135" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B42" s="136"/>
       <c r="C42" s="136"/>
@@ -12347,15 +12022,15 @@
         <v>7</v>
       </c>
       <c r="G42" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H42" s="56" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="27" thickBot="1">
       <c r="A43" s="139" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B43" s="140"/>
       <c r="C43" s="141"/>
@@ -12379,14 +12054,14 @@
         <v>8.3333333333333321</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="15.75" thickBot="1"/>
+    <row r="46" spans="1:8" ht="36.75" customHeight="1">
       <c r="A46" s="131" t="s">
         <v>28</v>
       </c>
       <c r="B46" s="132"/>
     </row>
-    <row r="47" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" ht="15.75">
       <c r="A47" s="22" t="s">
         <v>30</v>
       </c>
@@ -12394,7 +12069,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8">
       <c r="A48" s="20" t="s">
         <v>13</v>
       </c>
@@ -12403,7 +12078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2">
       <c r="A49" s="20" t="s">
         <v>14</v>
       </c>
@@ -12412,7 +12087,7 @@
         <v>16.666666666666664</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2">
       <c r="A50" s="20" t="s">
         <v>15</v>
       </c>
@@ -12422,17 +12097,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A39:H39"/>
-    <mergeCell ref="G40:H41"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="A46:B46"/>
     <mergeCell ref="A31:H31"/>
     <mergeCell ref="A1:L6"/>
     <mergeCell ref="A8:C9"/>
     <mergeCell ref="A15:J15"/>
     <mergeCell ref="A21:H21"/>
     <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A39:H39"/>
+    <mergeCell ref="G40:H41"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="A46:B46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -12564,15 +12239,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="100" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="101"/>
       <c r="C1" s="101"/>
@@ -12584,7 +12259,7 @@
       <c r="I1" s="101"/>
       <c r="J1" s="102"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" s="103"/>
       <c r="B2" s="104"/>
       <c r="C2" s="104"/>
@@ -12596,7 +12271,7 @@
       <c r="I2" s="104"/>
       <c r="J2" s="105"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" s="103"/>
       <c r="B3" s="104"/>
       <c r="C3" s="104"/>
@@ -12608,7 +12283,7 @@
       <c r="I3" s="104"/>
       <c r="J3" s="105"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" s="103"/>
       <c r="B4" s="104"/>
       <c r="C4" s="104"/>
@@ -12620,7 +12295,7 @@
       <c r="I4" s="104"/>
       <c r="J4" s="105"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" s="103"/>
       <c r="B5" s="104"/>
       <c r="C5" s="104"/>
@@ -12632,7 +12307,7 @@
       <c r="I5" s="104"/>
       <c r="J5" s="105"/>
     </row>
-    <row r="6" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1">
       <c r="A6" s="106"/>
       <c r="B6" s="107"/>
       <c r="C6" s="107"/>
@@ -12644,20 +12319,20 @@
       <c r="I6" s="107"/>
       <c r="J6" s="108"/>
     </row>
-    <row r="7" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="15.95" thickBot="1"/>
+    <row r="8" spans="1:10">
       <c r="A8" s="125" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B8" s="126"/>
       <c r="C8" s="127"/>
     </row>
-    <row r="9" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="33" customHeight="1" thickBot="1">
       <c r="A9" s="128"/>
       <c r="B9" s="129"/>
       <c r="C9" s="130"/>
     </row>
-    <row r="10" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="26.25" thickBot="1">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -12668,7 +12343,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="15.95" thickBot="1">
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
@@ -12679,7 +12354,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15.95" thickBot="1">
       <c r="A12" s="7" t="s">
         <v>23</v>
       </c>
@@ -12690,7 +12365,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15.95" thickBot="1">
       <c r="A13" s="10" t="s">
         <v>24</v>
       </c>
@@ -12701,10 +12376,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:10" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15.95" thickBot="1"/>
+    <row r="15" spans="1:10" ht="20.100000000000001" thickBot="1">
       <c r="A15" s="133" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" s="134"/>
       <c r="C15" s="134"/>
@@ -12712,32 +12387,32 @@
       <c r="E15" s="134"/>
       <c r="F15" s="134"/>
     </row>
-    <row r="16" spans="1:10" ht="25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="24.95" thickBot="1">
       <c r="A16" s="37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="65" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="63" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" s="40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E16" s="40" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F16" s="40" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="23.1" thickBot="1">
       <c r="A17" s="42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B17" s="43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C17" s="34" t="s">
         <v>12</v>
@@ -12753,10 +12428,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15.75" thickBot="1"/>
+    <row r="22" spans="1:6" ht="19.5" thickBot="1">
       <c r="A22" s="133" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B22" s="134"/>
       <c r="C22" s="134"/>
@@ -12764,32 +12439,32 @@
       <c r="E22" s="134"/>
       <c r="F22" s="134"/>
     </row>
-    <row r="23" spans="1:6" ht="25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="24.75" thickBot="1">
       <c r="A23" s="37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" s="65" t="s">
         <v>3</v>
       </c>
       <c r="C23" s="63" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D23" s="40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E23" s="40" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F23" s="40" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="30.75" thickBot="1">
       <c r="A24" s="42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B24" s="43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C24" s="34" t="s">
         <v>12</v>
@@ -12805,10 +12480,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15.75" thickBot="1"/>
+    <row r="27" spans="1:6" ht="19.5" thickBot="1">
       <c r="A27" s="133" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B27" s="134"/>
       <c r="C27" s="134"/>
@@ -12816,32 +12491,32 @@
       <c r="E27" s="134"/>
       <c r="F27" s="134"/>
     </row>
-    <row r="28" spans="1:6" ht="25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="24.75" thickBot="1">
       <c r="A28" s="37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28" s="90" t="s">
         <v>3</v>
       </c>
       <c r="C28" s="63" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D28" s="40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E28" s="40" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F28" s="40" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="30.75" thickBot="1">
       <c r="A29" s="42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B29" s="43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C29" s="34" t="s">
         <v>12</v>
@@ -12857,10 +12532,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="1:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="15.75" thickBot="1"/>
+    <row r="34" spans="1:14" ht="19.5" thickBot="1">
       <c r="A34" s="137" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B34" s="138"/>
       <c r="C34" s="138"/>
@@ -12873,15 +12548,15 @@
       <c r="M34" s="73"/>
       <c r="N34" s="73"/>
     </row>
-    <row r="35" spans="1:14" ht="25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="24.75" thickBot="1">
       <c r="A35" s="53" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" s="54" t="s">
         <v>3</v>
       </c>
       <c r="C35" s="54" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D35" s="54" t="s">
         <v>13</v>
@@ -12898,12 +12573,12 @@
       <c r="M35" s="73"/>
       <c r="N35" s="73"/>
     </row>
-    <row r="36" spans="1:14" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="53.25" customHeight="1" thickBot="1">
       <c r="A36" s="42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B36" s="43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C36" s="34" t="s">
         <v>12</v>
@@ -12923,9 +12598,9 @@
       <c r="M36" s="73"/>
       <c r="N36" s="73"/>
     </row>
-    <row r="37" spans="1:14" ht="24" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" ht="24">
       <c r="A37" s="135" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B37" s="136"/>
       <c r="C37" s="136"/>
@@ -12939,15 +12614,15 @@
         <v>0</v>
       </c>
       <c r="G37" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H37" s="56" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="27" thickBot="1">
       <c r="A38" s="147" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B38" s="148"/>
       <c r="C38" s="149"/>
@@ -12969,14 +12644,14 @@
         <v>14.333333333333334</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="15.75" thickBot="1"/>
+    <row r="44" spans="1:14" ht="18.75">
       <c r="A44" s="131" t="s">
         <v>28</v>
       </c>
       <c r="B44" s="132"/>
     </row>
-    <row r="45" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" ht="15.75">
       <c r="A45" s="22" t="s">
         <v>30</v>
       </c>
@@ -12984,7 +12659,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14">
       <c r="A46" s="64" t="s">
         <v>13</v>
       </c>
@@ -12992,7 +12667,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14">
       <c r="A47" s="64" t="s">
         <v>14</v>
       </c>
@@ -13000,7 +12675,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14">
       <c r="A48" s="64" t="s">
         <v>15</v>
       </c>
@@ -13116,21 +12791,21 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="11.5" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" customWidth="1"/>
-    <col min="6" max="7" width="8.1640625" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" customWidth="1"/>
-    <col min="9" max="9" width="9.5" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" customWidth="1"/>
-    <col min="11" max="11" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="7" width="8.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" ht="15" customHeight="1">
       <c r="A1" s="100" t="s">
         <v>0</v>
       </c>
@@ -13153,7 +12828,7 @@
       <c r="R1" s="33"/>
       <c r="S1" s="33"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="103"/>
       <c r="B2" s="104"/>
       <c r="C2" s="104"/>
@@ -13174,7 +12849,7 @@
       <c r="R2" s="33"/>
       <c r="S2" s="33"/>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="103"/>
       <c r="B3" s="104"/>
       <c r="C3" s="104"/>
@@ -13195,7 +12870,7 @@
       <c r="R3" s="33"/>
       <c r="S3" s="33"/>
     </row>
-    <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="15" customHeight="1">
       <c r="A4" s="103"/>
       <c r="B4" s="104"/>
       <c r="C4" s="104"/>
@@ -13216,7 +12891,7 @@
       <c r="R4" s="33"/>
       <c r="S4" s="33"/>
     </row>
-    <row r="5" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" ht="15.75" customHeight="1">
       <c r="A5" s="103"/>
       <c r="B5" s="104"/>
       <c r="C5" s="104"/>
@@ -13237,7 +12912,7 @@
       <c r="R5" s="33"/>
       <c r="S5" s="33"/>
     </row>
-    <row r="6" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="15.75" customHeight="1" thickBot="1">
       <c r="A6" s="106"/>
       <c r="B6" s="107"/>
       <c r="C6" s="107"/>
@@ -13258,20 +12933,20 @@
       <c r="R6" s="33"/>
       <c r="S6" s="33"/>
     </row>
-    <row r="7" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" ht="15.95" thickBot="1"/>
+    <row r="8" spans="1:19">
       <c r="C8" s="125" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D8" s="126"/>
       <c r="E8" s="127"/>
     </row>
-    <row r="9" spans="1:19" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="23.25" customHeight="1" thickBot="1">
       <c r="C9" s="128"/>
       <c r="D9" s="129"/>
       <c r="E9" s="130"/>
     </row>
-    <row r="10" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="26.25" thickBot="1">
       <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
@@ -13282,7 +12957,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="15.95" thickBot="1">
       <c r="C11" s="3" t="s">
         <v>22</v>
       </c>
@@ -13293,7 +12968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="15.95" thickBot="1">
       <c r="C12" s="7" t="s">
         <v>23</v>
       </c>
@@ -13304,7 +12979,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="15.95" thickBot="1">
       <c r="C13" s="10" t="s">
         <v>24</v>
       </c>
@@ -13315,10 +12990,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:19" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="15.95" thickBot="1"/>
+    <row r="15" spans="1:19" ht="32.25" customHeight="1" thickBot="1">
       <c r="A15" s="133" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" s="134"/>
       <c r="C15" s="134"/>
@@ -13331,27 +13006,27 @@
       <c r="J15" s="48"/>
       <c r="K15" s="48"/>
     </row>
-    <row r="16" spans="1:19" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="48.95" thickBot="1">
       <c r="A16" s="37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="82" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" s="40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E16" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="40" t="s">
+      <c r="G16" s="40" t="s">
         <v>58</v>
-      </c>
-      <c r="G16" s="40" t="s">
-        <v>59</v>
       </c>
       <c r="H16" s="40" t="s">
         <v>17</v>
@@ -13360,7 +13035,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="43" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="51.75" thickBot="1">
       <c r="A17" s="42" t="s">
         <v>2</v>
       </c>
@@ -13368,7 +13043,7 @@
         <v>6</v>
       </c>
       <c r="C17" s="44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D17" s="45" t="s">
         <v>13</v>
@@ -13391,10 +13066,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:11" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="15.95" thickBot="1"/>
+    <row r="20" spans="1:11" ht="30.75" customHeight="1" thickBot="1">
       <c r="A20" s="133" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B20" s="134"/>
       <c r="C20" s="134"/>
@@ -13405,27 +13080,27 @@
       <c r="H20" s="134"/>
       <c r="I20" s="134"/>
     </row>
-    <row r="21" spans="1:11" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="48.75" customHeight="1" thickBot="1">
       <c r="A21" s="37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" s="82" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D21" s="40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E21" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="F21" s="40" t="s">
+      <c r="G21" s="40" t="s">
         <v>58</v>
-      </c>
-      <c r="G21" s="40" t="s">
-        <v>59</v>
       </c>
       <c r="H21" s="40" t="s">
         <v>17</v>
@@ -13434,7 +13109,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="43" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="51.75" thickBot="1">
       <c r="A22" s="42" t="s">
         <v>2</v>
       </c>
@@ -13442,7 +13117,7 @@
         <v>6</v>
       </c>
       <c r="C22" s="44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D22" s="45" t="s">
         <v>14</v>
@@ -13465,7 +13140,7 @@
         <v>0.21621621621621623</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="33.75" customHeight="1" thickBot="1">
       <c r="A23" s="51"/>
       <c r="B23" s="84"/>
       <c r="C23" s="85"/>
@@ -13476,9 +13151,9 @@
       <c r="H23" s="87"/>
       <c r="I23" s="87"/>
     </row>
-    <row r="24" spans="1:11" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="30.75" customHeight="1" thickBot="1">
       <c r="A24" s="133" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B24" s="134"/>
       <c r="C24" s="134"/>
@@ -13489,27 +13164,27 @@
       <c r="H24" s="134"/>
       <c r="I24" s="134"/>
     </row>
-    <row r="25" spans="1:11" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="48.75" customHeight="1" thickBot="1">
       <c r="A25" s="37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B25" s="82" t="s">
         <v>3</v>
       </c>
       <c r="C25" s="39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D25" s="40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E25" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="F25" s="40" t="s">
+      <c r="G25" s="40" t="s">
         <v>58</v>
-      </c>
-      <c r="G25" s="40" t="s">
-        <v>59</v>
       </c>
       <c r="H25" s="40" t="s">
         <v>17</v>
@@ -13518,7 +13193,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="43" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="51.75" thickBot="1">
       <c r="A26" s="42" t="s">
         <v>2</v>
       </c>
@@ -13526,7 +13201,7 @@
         <v>6</v>
       </c>
       <c r="C26" s="44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D26" s="45" t="s">
         <v>15</v>
@@ -13549,7 +13224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="21" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="21">
       <c r="A27" s="51"/>
       <c r="B27" s="84"/>
       <c r="C27" s="85"/>
@@ -13560,10 +13235,10 @@
       <c r="H27" s="87"/>
       <c r="I27" s="87"/>
     </row>
-    <row r="28" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:11" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="15.75" thickBot="1"/>
+    <row r="29" spans="1:11" ht="42.75" customHeight="1" thickBot="1">
       <c r="A29" s="133" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B29" s="134"/>
       <c r="C29" s="134"/>
@@ -13576,15 +13251,15 @@
       <c r="J29" s="48"/>
       <c r="K29" s="48"/>
     </row>
-    <row r="30" spans="1:11" s="31" customFormat="1" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" s="31" customFormat="1" ht="45.75" customHeight="1" thickBot="1">
       <c r="A30" s="53" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" s="54" t="s">
         <v>3</v>
       </c>
       <c r="C30" s="54" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D30" s="54" t="s">
         <v>13</v>
@@ -13601,7 +13276,7 @@
       <c r="J30" s="50"/>
       <c r="K30" s="50"/>
     </row>
-    <row r="31" spans="1:11" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="39" customHeight="1" thickBot="1">
       <c r="A31" s="57" t="s">
         <v>2</v>
       </c>
@@ -13609,7 +13284,7 @@
         <v>6</v>
       </c>
       <c r="C31" s="44" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D31" s="13">
         <v>0</v>
@@ -13626,9 +13301,9 @@
       <c r="J31" s="51"/>
       <c r="K31" s="52"/>
     </row>
-    <row r="32" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="28.5" customHeight="1">
       <c r="A32" s="150" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B32" s="151"/>
       <c r="C32" s="151"/>
@@ -13643,15 +13318,15 @@
       </c>
       <c r="G32" s="151"/>
       <c r="H32" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I32" s="56" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" ht="27" thickBot="1">
       <c r="A33" s="139" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B33" s="140"/>
       <c r="C33" s="141"/>
@@ -13677,11 +13352,11 @@
         <v>7.2072072072072071E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:21">
       <c r="L34" s="58"/>
     </row>
-    <row r="38" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:21" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" ht="15.75" thickBot="1"/>
+    <row r="39" spans="1:21" ht="39.75" customHeight="1">
       <c r="B39" s="131" t="s">
         <v>28</v>
       </c>
@@ -13696,7 +13371,7 @@
       <c r="K39" s="21"/>
       <c r="U39" s="49"/>
     </row>
-    <row r="40" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:21" ht="15.75">
       <c r="B40" s="22" t="s">
         <v>30</v>
       </c>
@@ -13704,7 +13379,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:21">
       <c r="B41" s="81" t="s">
         <v>13</v>
       </c>
@@ -13713,7 +13388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:21">
       <c r="B42" s="81" t="s">
         <v>14</v>
       </c>
@@ -13722,7 +13397,7 @@
         <v>0.21621621621621623</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:21">
       <c r="B43" s="81" t="s">
         <v>15</v>
       </c>
@@ -13733,6 +13408,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A29:I29"/>
+    <mergeCell ref="A1:M6"/>
+    <mergeCell ref="C8:E9"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="A20:I20"/>
+    <mergeCell ref="A24:I24"/>
     <mergeCell ref="H30:I31"/>
     <mergeCell ref="A32:C32"/>
     <mergeCell ref="A33:C33"/>
@@ -13741,12 +13422,6 @@
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="F32:G32"/>
     <mergeCell ref="F33:G33"/>
-    <mergeCell ref="A29:I29"/>
-    <mergeCell ref="A1:M6"/>
-    <mergeCell ref="C8:E9"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="A20:I20"/>
-    <mergeCell ref="A24:I24"/>
   </mergeCells>
   <conditionalFormatting sqref="J31">
     <cfRule type="iconSet" priority="4">
@@ -13870,7 +13545,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
correciones PPQA, archivos CM
</commit_message>
<xml_diff>
--- a/Area de proceso MA/TABME_V1.0_2017.xlsx
+++ b/Area de proceso MA/TABME_V1.0_2017.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DESAROLLO\documentationStaradmin-master\Area de proceso MA\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="10185" yWindow="2520" windowWidth="20505" windowHeight="7665" activeTab="1"/>
   </bookViews>
@@ -19,7 +14,7 @@
     <sheet name="FMICIC" sheetId="10" state="hidden" r:id="rId5"/>
     <sheet name="Hoja1" sheetId="11" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1500,7 +1495,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-PE"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1517,12 +1512,9 @@
             <c:strRef>
               <c:f>FMNCONPRO!$B$31:$C$31</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PPQA</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Numero de N conformidades QA del Producto</c:v>
+                  <c:v>PPQA Numero de N conformidades QA del Producto</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1573,7 +1565,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-PE"/>
+                <a:endParaRPr lang="es-ES"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -1631,7 +1623,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1657,11 +1649,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="259137744"/>
-        <c:axId val="259138920"/>
+        <c:axId val="40217984"/>
+        <c:axId val="52628096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="259137744"/>
+        <c:axId val="40217984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1702,26 +1694,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-PE"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1757,10 +1729,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-PE"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="259138920"/>
+        <c:crossAx val="52628096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1768,7 +1740,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="259138920"/>
+        <c:axId val="52628096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1835,32 +1807,12 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-PE"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="259137744"/>
+        <c:crossAx val="40217984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1914,7 +1866,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-PE"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1981,26 +1933,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-PE"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -2016,12 +1948,9 @@
             <c:strRef>
               <c:f>FMNCONPRO!$C$39:$C$40</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TABLERO DE METRICAS DE N CONFORMIDADES QA DE PRODUCTO</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>VALORES</c:v>
+                  <c:v>TABLERO DE METRICAS DE N CONFORMIDADES QA DE PRODUCTO VALORES</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2067,7 +1996,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-PE"/>
+                <a:endParaRPr lang="es-ES"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="inEnd"/>
@@ -2125,7 +2054,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2149,11 +2078,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="259139704"/>
-        <c:axId val="259140096"/>
+        <c:axId val="52668672"/>
+        <c:axId val="52679808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="259139704"/>
+        <c:axId val="52668672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2193,10 +2122,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-PE"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="259140096"/>
+        <c:crossAx val="52679808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2204,7 +2133,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="259140096"/>
+        <c:axId val="52679808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2225,7 +2154,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="259139704"/>
+        <c:crossAx val="52668672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2276,7 +2205,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-PE"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2332,6 +2261,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2340,26 +2270,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-PE"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -2459,11 +2369,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="259140880"/>
-        <c:axId val="259141272"/>
+        <c:axId val="160216192"/>
+        <c:axId val="160218496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="259140880"/>
+        <c:axId val="160216192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2495,6 +2405,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2503,26 +2414,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-PE"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2558,10 +2449,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-PE"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="259141272"/>
+        <c:crossAx val="160218496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2569,7 +2460,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="259141272"/>
+        <c:axId val="160218496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2615,6 +2506,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2623,26 +2515,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-PE"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2672,10 +2544,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-PE"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="259140880"/>
+        <c:crossAx val="160216192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2689,6 +2561,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="1"/>
       <c:spPr>
         <a:noFill/>
@@ -2717,7 +2590,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-PE"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2744,7 +2617,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-PE"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2803,7 +2676,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-PE"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2860,12 +2733,9 @@
             <c:strRef>
               <c:f>FMVREQM!$B$46:$B$47</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TABLERO DE METRICAS DE N CONFORMIDADES QA DE PRODUCTO</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>VALORES</c:v>
+                  <c:v>TABLERO DE METRICAS DE N CONFORMIDADES QA DE PRODUCTO VALORES</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2932,12 +2802,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="259142056"/>
-        <c:axId val="259142448"/>
+        <c:axId val="160248576"/>
+        <c:axId val="160250112"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="259142056"/>
+        <c:axId val="160248576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2971,10 +2841,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-PE"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="259142448"/>
+        <c:crossAx val="160250112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2982,7 +2852,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="259142448"/>
+        <c:axId val="160250112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3027,10 +2897,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-PE"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="259142056"/>
+        <c:crossAx val="160248576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3065,7 +2935,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-PE"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3116,6 +2986,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3124,26 +2995,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-PE"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -3200,7 +3051,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-PE"/>
+                <a:endParaRPr lang="es-ES"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -3283,11 +3134,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="260626120"/>
-        <c:axId val="260626512"/>
+        <c:axId val="169944960"/>
+        <c:axId val="169981056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="260626120"/>
+        <c:axId val="169944960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3324,6 +3175,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3332,26 +3184,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-PE"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -3387,10 +3219,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-PE"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="260626512"/>
+        <c:crossAx val="169981056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3398,7 +3230,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="260626512"/>
+        <c:axId val="169981056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3446,6 +3278,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3454,32 +3287,12 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-PE"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="260626120"/>
+        <c:crossAx val="169944960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3530,7 +3343,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-PE"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3587,6 +3400,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3595,32 +3409,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-PE"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -3733,11 +3521,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="260627688"/>
-        <c:axId val="260628080"/>
+        <c:axId val="170017920"/>
+        <c:axId val="170019840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="260627688"/>
+        <c:axId val="170017920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3768,6 +3556,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3776,25 +3565,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="85000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-PE"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -3829,10 +3599,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-PE"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="260628080"/>
+        <c:crossAx val="170019840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3840,7 +3610,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="260628080"/>
+        <c:axId val="170019840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3885,6 +3655,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3893,25 +3664,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="85000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-PE"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -3940,10 +3692,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-PE"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="260627688"/>
+        <c:crossAx val="170017920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3994,7 +3746,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-PE"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4053,7 +3805,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-PE"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4070,12 +3822,9 @@
             <c:strRef>
               <c:f>FMICIC!$B$31:$C$31</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CM</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Numero de Items Modificados</c:v>
+                  <c:v>CM Numero de Items Modificados</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4126,7 +3875,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-PE"/>
+                <a:endParaRPr lang="es-ES"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -4209,11 +3958,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="260628864"/>
-        <c:axId val="260629256"/>
+        <c:axId val="170060800"/>
+        <c:axId val="170141952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="260628864"/>
+        <c:axId val="170060800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4253,26 +4002,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-PE"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -4308,10 +4037,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-PE"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="260629256"/>
+        <c:crossAx val="170141952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4319,7 +4048,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="260629256"/>
+        <c:axId val="170141952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4385,32 +4114,12 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-PE"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="260628864"/>
+        <c:crossAx val="170060800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4464,7 +4173,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-PE"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4531,26 +4240,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-PE"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -4566,12 +4255,9 @@
             <c:strRef>
               <c:f>FMICIC!$C$39:$C$40</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TABLERO DE METRICAS DE N CONFORMIDADES QA DE PRODUCTO</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>VALORES</c:v>
+                  <c:v>TABLERO DE METRICAS DE N CONFORMIDADES QA DE PRODUCTO VALORES</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4617,7 +4303,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-PE"/>
+                <a:endParaRPr lang="es-ES"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="inEnd"/>
@@ -4698,11 +4384,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="260627296"/>
-        <c:axId val="260630040"/>
+        <c:axId val="170166144"/>
+        <c:axId val="159187712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="260627296"/>
+        <c:axId val="170166144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4742,10 +4428,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-PE"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="260630040"/>
+        <c:crossAx val="159187712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4753,7 +4439,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="260630040"/>
+        <c:axId val="159187712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4774,7 +4460,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="260627296"/>
+        <c:crossAx val="170166144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4825,7 +4511,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-PE"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -10482,7 +10168,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -10887,7 +10573,7 @@
       </c>
       <c r="M20" s="88">
         <f>FMNCONPRO!E33</f>
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="N20" s="88">
         <f>FMNCONPRO!F33</f>
@@ -10899,7 +10585,7 @@
       </c>
       <c r="P20" s="88">
         <f>FMNCONPRO!H33</f>
-        <v>6.6666666666666666E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="0.75" hidden="1" customHeight="1">
@@ -11099,8 +10785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -11571,7 +11257,7 @@
         <v>0</v>
       </c>
       <c r="E31" s="13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F31" s="13">
         <v>0</v>
@@ -11615,7 +11301,7 @@
       </c>
       <c r="E33" s="59">
         <f>E31/E32</f>
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="F33" s="89">
         <f>F31/F32</f>
@@ -11627,7 +11313,7 @@
       </c>
       <c r="H33" s="62">
         <f>AVERAGE(D33:F33)</f>
-        <v>6.6666666666666666E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="34" spans="1:20">
@@ -11671,7 +11357,7 @@
       </c>
       <c r="C42" s="36">
         <f>E31/E32</f>
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="43" spans="1:20">
@@ -11816,8 +11502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -12416,17 +12102,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A39:H39"/>
+    <mergeCell ref="G40:H41"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="A46:B46"/>
     <mergeCell ref="A31:H31"/>
     <mergeCell ref="A1:L6"/>
     <mergeCell ref="A8:C9"/>
     <mergeCell ref="A15:J15"/>
     <mergeCell ref="A21:H21"/>
     <mergeCell ref="A27:H27"/>
-    <mergeCell ref="A39:H39"/>
-    <mergeCell ref="G40:H41"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="A46:B46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -12558,8 +12244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -13727,12 +13413,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A29:I29"/>
-    <mergeCell ref="A1:M6"/>
-    <mergeCell ref="C8:E9"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="A20:I20"/>
-    <mergeCell ref="A24:I24"/>
     <mergeCell ref="H30:I31"/>
     <mergeCell ref="A32:C32"/>
     <mergeCell ref="A33:C33"/>
@@ -13741,6 +13421,12 @@
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="F32:G32"/>
     <mergeCell ref="F33:G33"/>
+    <mergeCell ref="A29:I29"/>
+    <mergeCell ref="A1:M6"/>
+    <mergeCell ref="C8:E9"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="A20:I20"/>
+    <mergeCell ref="A24:I24"/>
   </mergeCells>
   <conditionalFormatting sqref="J31">
     <cfRule type="iconSet" priority="4">

</xml_diff>